<commit_message>
update data and rds files
</commit_message>
<xml_diff>
--- a/data/Shorezone_coastal-classes.xlsx
+++ b/data/Shorezone_coastal-classes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chguo/nearshore-fish/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDB5DB6-DA54-2C44-8ABB-DE158166E4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1528C16-5B69-784F-B339-3D62F6AF67EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9740" yWindow="-24880" windowWidth="21120" windowHeight="19440" xr2:uid="{451A1F88-5C4B-0C49-9BAD-892D9FFBC099}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{451A1F88-5C4B-0C49-9BAD-892D9FFBC099}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="62">
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>Structuring_process</t>
   </si>
   <si>
@@ -222,6 +219,9 @@
   </si>
   <si>
     <t>Steep</t>
+  </si>
+  <si>
+    <t>SHORETYPE</t>
   </si>
 </sst>
 </file>
@@ -257,13 +257,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -284,9 +280,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -324,7 +320,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -430,7 +426,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -572,7 +568,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -582,9 +578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8977F357-87CE-8B40-A4A1-68F6DB67C043}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -599,22 +593,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -622,19 +616,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -642,19 +636,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -662,19 +656,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -682,19 +676,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -702,19 +696,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -722,19 +716,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -742,19 +736,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -762,19 +756,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -782,19 +776,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -802,19 +796,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -822,19 +816,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -842,19 +836,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -862,16 +856,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -879,16 +873,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -896,16 +890,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -913,19 +907,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -933,19 +927,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -953,19 +947,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -973,19 +967,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -993,19 +987,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1013,19 +1007,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1033,19 +1027,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1053,19 +1047,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1073,19 +1067,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1093,19 +1087,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1113,19 +1107,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1133,19 +1127,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1153,19 +1147,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1173,19 +1167,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1193,19 +1187,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1213,10 +1207,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1224,10 +1218,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>11</v>
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1235,10 +1229,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1246,10 +1240,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1257,10 +1251,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1268,10 +1262,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>15</v>
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1279,10 +1273,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1290,10 +1284,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1301,10 +1295,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>